<commit_message>
Redoing taxonomy with tol, making changes to units in spreadsheet, removing duplicate sources and formtting original source columns
</commit_message>
<xml_diff>
--- a/Raw_data/master_length_weight.xlsx
+++ b/Raw_data/master_length_weight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/My Drive/R/Biovolume database/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616DCC0A-A1F8-C645-A417-AD7E5963D0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504AE43C-5676-0D4B-AE5E-B96916EC01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
   </bookViews>
   <sheets>
     <sheet name="McCauley" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="186">
   <si>
     <t>subclass</t>
   </si>
@@ -522,66 +522,6 @@
     <t>0.4*abc</t>
   </si>
   <si>
-    <t>anuraeopsis</t>
-  </si>
-  <si>
-    <t>ascomorpha</t>
-  </si>
-  <si>
-    <t>asplanchna</t>
-  </si>
-  <si>
-    <t>brachionus</t>
-  </si>
-  <si>
-    <t>conochilus</t>
-  </si>
-  <si>
-    <t>collotheca</t>
-  </si>
-  <si>
-    <t>euchlanis</t>
-  </si>
-  <si>
-    <t>filinia</t>
-  </si>
-  <si>
-    <t>gastropus</t>
-  </si>
-  <si>
-    <t>hexarthra</t>
-  </si>
-  <si>
-    <t>kellikottia</t>
-  </si>
-  <si>
-    <t>keratella quadrata</t>
-  </si>
-  <si>
-    <t>keratella cochlearis</t>
-  </si>
-  <si>
-    <t>notholca</t>
-  </si>
-  <si>
-    <t>ploesoma</t>
-  </si>
-  <si>
-    <t>polyarthra</t>
-  </si>
-  <si>
-    <t>pompbolyx</t>
-  </si>
-  <si>
-    <t>synchaeta</t>
-  </si>
-  <si>
-    <t>testudinella</t>
-  </si>
-  <si>
-    <t>trichocerca</t>
-  </si>
-  <si>
     <t>daphnia magna</t>
   </si>
   <si>
@@ -601,6 +541,66 @@
   </si>
   <si>
     <t>org.genus</t>
+  </si>
+  <si>
+    <t>Anuraeopsis</t>
+  </si>
+  <si>
+    <t>Ascomorpha</t>
+  </si>
+  <si>
+    <t>Asplanchna</t>
+  </si>
+  <si>
+    <t>Brachionus</t>
+  </si>
+  <si>
+    <t>Conochilus</t>
+  </si>
+  <si>
+    <t>Collotheca</t>
+  </si>
+  <si>
+    <t>Euchlanis</t>
+  </si>
+  <si>
+    <t>Filinia</t>
+  </si>
+  <si>
+    <t>Gastropus</t>
+  </si>
+  <si>
+    <t>Hexarthra</t>
+  </si>
+  <si>
+    <t>Kellikottia</t>
+  </si>
+  <si>
+    <t>Keratella quadrata</t>
+  </si>
+  <si>
+    <t>Keratella cochlearis</t>
+  </si>
+  <si>
+    <t>Notholca</t>
+  </si>
+  <si>
+    <t>Ploesoma</t>
+  </si>
+  <si>
+    <t>Polyarthra</t>
+  </si>
+  <si>
+    <t>Pompbolyx</t>
+  </si>
+  <si>
+    <t>Synchaeta</t>
+  </si>
+  <si>
+    <t>Testudinella</t>
+  </si>
+  <si>
+    <t>Trichocerca</t>
   </si>
 </sst>
 </file>
@@ -992,16 +992,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E21" s="1">
         <v>1.6729000000000001</v>
@@ -1591,7 +1591,7 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E22" s="1">
         <v>1.8268</v>
@@ -1623,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E23" s="1">
         <v>2.2000000000000002</v>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E24" s="1">
         <v>2.5099999999999998</v>
@@ -1673,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E25" s="1">
         <v>2.36</v>
@@ -1697,7 +1697,7 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E26" s="1">
         <v>2.12</v>
@@ -3532,240 +3532,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0B2460-2955-5C43-9837-B1D9B7377E5B}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>148</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2">
         <v>0.33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3">
         <v>0.52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4">
         <v>0.52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5">
         <v>0.52</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6">
         <v>0.26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7">
         <v>0.26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8">
         <v>0.52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9">
         <v>0.52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10">
         <v>0.8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11">
         <v>0.26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12">
         <v>0.26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>171</v>
-      </c>
-      <c r="B14">
+        <v>178</v>
+      </c>
+      <c r="C14">
         <v>0.13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15">
         <v>0.13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16">
         <v>0.52</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18">
         <v>0.4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19">
         <v>0.26</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20">
         <v>0.4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21">
         <v>0.52</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4974,7 +4977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970E19EB-C40E-1344-9A19-A1BB7A0CCA20}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4982,7 +4985,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5061,7 +5064,7 @@
         <v>2.399</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating all the folders
</commit_message>
<xml_diff>
--- a/Raw_data/master_length_weight.xlsx
+++ b/Raw_data/master_length_weight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/Raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/My Drive/R/Biovolume database/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504AE43C-5676-0D4B-AE5E-B96916EC01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616DCC0A-A1F8-C645-A417-AD7E5963D0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
+    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
   </bookViews>
   <sheets>
     <sheet name="McCauley" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="186">
   <si>
     <t>subclass</t>
   </si>
@@ -522,6 +522,66 @@
     <t>0.4*abc</t>
   </si>
   <si>
+    <t>anuraeopsis</t>
+  </si>
+  <si>
+    <t>ascomorpha</t>
+  </si>
+  <si>
+    <t>asplanchna</t>
+  </si>
+  <si>
+    <t>brachionus</t>
+  </si>
+  <si>
+    <t>conochilus</t>
+  </si>
+  <si>
+    <t>collotheca</t>
+  </si>
+  <si>
+    <t>euchlanis</t>
+  </si>
+  <si>
+    <t>filinia</t>
+  </si>
+  <si>
+    <t>gastropus</t>
+  </si>
+  <si>
+    <t>hexarthra</t>
+  </si>
+  <si>
+    <t>kellikottia</t>
+  </si>
+  <si>
+    <t>keratella quadrata</t>
+  </si>
+  <si>
+    <t>keratella cochlearis</t>
+  </si>
+  <si>
+    <t>notholca</t>
+  </si>
+  <si>
+    <t>ploesoma</t>
+  </si>
+  <si>
+    <t>polyarthra</t>
+  </si>
+  <si>
+    <t>pompbolyx</t>
+  </si>
+  <si>
+    <t>synchaeta</t>
+  </si>
+  <si>
+    <t>testudinella</t>
+  </si>
+  <si>
+    <t>trichocerca</t>
+  </si>
+  <si>
     <t>daphnia magna</t>
   </si>
   <si>
@@ -541,66 +601,6 @@
   </si>
   <si>
     <t>org.genus</t>
-  </si>
-  <si>
-    <t>Anuraeopsis</t>
-  </si>
-  <si>
-    <t>Ascomorpha</t>
-  </si>
-  <si>
-    <t>Asplanchna</t>
-  </si>
-  <si>
-    <t>Brachionus</t>
-  </si>
-  <si>
-    <t>Conochilus</t>
-  </si>
-  <si>
-    <t>Collotheca</t>
-  </si>
-  <si>
-    <t>Euchlanis</t>
-  </si>
-  <si>
-    <t>Filinia</t>
-  </si>
-  <si>
-    <t>Gastropus</t>
-  </si>
-  <si>
-    <t>Hexarthra</t>
-  </si>
-  <si>
-    <t>Kellikottia</t>
-  </si>
-  <si>
-    <t>Keratella quadrata</t>
-  </si>
-  <si>
-    <t>Keratella cochlearis</t>
-  </si>
-  <si>
-    <t>Notholca</t>
-  </si>
-  <si>
-    <t>Ploesoma</t>
-  </si>
-  <si>
-    <t>Polyarthra</t>
-  </si>
-  <si>
-    <t>Pompbolyx</t>
-  </si>
-  <si>
-    <t>Synchaeta</t>
-  </si>
-  <si>
-    <t>Testudinella</t>
-  </si>
-  <si>
-    <t>Trichocerca</t>
   </si>
 </sst>
 </file>
@@ -992,16 +992,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E21" s="1">
         <v>1.6729000000000001</v>
@@ -1591,7 +1591,7 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E22" s="1">
         <v>1.8268</v>
@@ -1623,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E23" s="1">
         <v>2.2000000000000002</v>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E24" s="1">
         <v>2.5099999999999998</v>
@@ -1673,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E25" s="1">
         <v>2.36</v>
@@ -1697,7 +1697,7 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E26" s="1">
         <v>2.12</v>
@@ -3532,243 +3532,240 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0B2460-2955-5C43-9837-B1D9B7377E5B}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2">
+        <v>0.33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>0.52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <v>0.52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5">
+        <v>0.52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6">
+        <v>0.26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7">
+        <v>0.26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8">
+        <v>0.52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>166</v>
       </c>
-      <c r="C2">
-        <v>0.33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B9">
+        <v>0.52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>167</v>
       </c>
-      <c r="C3">
+      <c r="B10">
+        <v>0.8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11">
+        <v>0.26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12">
+        <v>0.26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14">
+        <v>0.13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15">
+        <v>0.13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16">
         <v>0.52</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18">
+        <v>0.4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19">
+        <v>0.26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20">
+        <v>0.4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21">
         <v>0.52</v>
       </c>
-      <c r="D4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5">
-        <v>0.52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6">
-        <v>0.26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7">
-        <v>0.26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8">
-        <v>0.52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C9">
-        <v>0.52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10">
-        <v>0.8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11">
-        <v>0.26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12">
-        <v>0.26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14">
-        <v>0.13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15">
-        <v>0.13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16">
-        <v>0.52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18">
-        <v>0.4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19">
-        <v>0.26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C20">
-        <v>0.4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>185</v>
-      </c>
-      <c r="C21">
-        <v>0.52</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4977,7 +4974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970E19EB-C40E-1344-9A19-A1BB7A0CCA20}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4985,7 +4982,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5064,7 +5061,7 @@
         <v>2.399</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replacing all folders because it went back to old one and I don't know why. This should be the most up to date version of everything now
</commit_message>
<xml_diff>
--- a/Raw_data/master_length_weight.xlsx
+++ b/Raw_data/master_length_weight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/My Drive/R/Biovolume database/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616DCC0A-A1F8-C645-A417-AD7E5963D0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504AE43C-5676-0D4B-AE5E-B96916EC01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
   </bookViews>
   <sheets>
     <sheet name="McCauley" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="186">
   <si>
     <t>subclass</t>
   </si>
@@ -522,66 +522,6 @@
     <t>0.4*abc</t>
   </si>
   <si>
-    <t>anuraeopsis</t>
-  </si>
-  <si>
-    <t>ascomorpha</t>
-  </si>
-  <si>
-    <t>asplanchna</t>
-  </si>
-  <si>
-    <t>brachionus</t>
-  </si>
-  <si>
-    <t>conochilus</t>
-  </si>
-  <si>
-    <t>collotheca</t>
-  </si>
-  <si>
-    <t>euchlanis</t>
-  </si>
-  <si>
-    <t>filinia</t>
-  </si>
-  <si>
-    <t>gastropus</t>
-  </si>
-  <si>
-    <t>hexarthra</t>
-  </si>
-  <si>
-    <t>kellikottia</t>
-  </si>
-  <si>
-    <t>keratella quadrata</t>
-  </si>
-  <si>
-    <t>keratella cochlearis</t>
-  </si>
-  <si>
-    <t>notholca</t>
-  </si>
-  <si>
-    <t>ploesoma</t>
-  </si>
-  <si>
-    <t>polyarthra</t>
-  </si>
-  <si>
-    <t>pompbolyx</t>
-  </si>
-  <si>
-    <t>synchaeta</t>
-  </si>
-  <si>
-    <t>testudinella</t>
-  </si>
-  <si>
-    <t>trichocerca</t>
-  </si>
-  <si>
     <t>daphnia magna</t>
   </si>
   <si>
@@ -601,6 +541,66 @@
   </si>
   <si>
     <t>org.genus</t>
+  </si>
+  <si>
+    <t>Anuraeopsis</t>
+  </si>
+  <si>
+    <t>Ascomorpha</t>
+  </si>
+  <si>
+    <t>Asplanchna</t>
+  </si>
+  <si>
+    <t>Brachionus</t>
+  </si>
+  <si>
+    <t>Conochilus</t>
+  </si>
+  <si>
+    <t>Collotheca</t>
+  </si>
+  <si>
+    <t>Euchlanis</t>
+  </si>
+  <si>
+    <t>Filinia</t>
+  </si>
+  <si>
+    <t>Gastropus</t>
+  </si>
+  <si>
+    <t>Hexarthra</t>
+  </si>
+  <si>
+    <t>Kellikottia</t>
+  </si>
+  <si>
+    <t>Keratella quadrata</t>
+  </si>
+  <si>
+    <t>Keratella cochlearis</t>
+  </si>
+  <si>
+    <t>Notholca</t>
+  </si>
+  <si>
+    <t>Ploesoma</t>
+  </si>
+  <si>
+    <t>Polyarthra</t>
+  </si>
+  <si>
+    <t>Pompbolyx</t>
+  </si>
+  <si>
+    <t>Synchaeta</t>
+  </si>
+  <si>
+    <t>Testudinella</t>
+  </si>
+  <si>
+    <t>Trichocerca</t>
   </si>
 </sst>
 </file>
@@ -992,16 +992,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E21" s="1">
         <v>1.6729000000000001</v>
@@ -1591,7 +1591,7 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E22" s="1">
         <v>1.8268</v>
@@ -1623,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E23" s="1">
         <v>2.2000000000000002</v>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E24" s="1">
         <v>2.5099999999999998</v>
@@ -1673,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E25" s="1">
         <v>2.36</v>
@@ -1697,7 +1697,7 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E26" s="1">
         <v>2.12</v>
@@ -3532,240 +3532,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0B2460-2955-5C43-9837-B1D9B7377E5B}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>148</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2">
         <v>0.33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3">
         <v>0.52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4">
         <v>0.52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5">
         <v>0.52</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6">
         <v>0.26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7">
         <v>0.26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8">
         <v>0.52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9">
         <v>0.52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10">
         <v>0.8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11">
         <v>0.26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12">
         <v>0.26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>171</v>
-      </c>
-      <c r="B14">
+        <v>178</v>
+      </c>
+      <c r="C14">
         <v>0.13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15">
         <v>0.13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16">
         <v>0.52</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18">
         <v>0.4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19">
         <v>0.26</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20">
         <v>0.4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21">
         <v>0.52</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4974,7 +4977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970E19EB-C40E-1344-9A19-A1BB7A0CCA20}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4982,7 +4985,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5061,7 +5064,7 @@
         <v>2.399</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redone the phylogeny maps
</commit_message>
<xml_diff>
--- a/Raw_data/master_length_weight.xlsx
+++ b/Raw_data/master_length_weight.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/Raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504AE43C-5676-0D4B-AE5E-B96916EC01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF06389-4A1E-694F-A904-059C36AA29F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
   </bookViews>
   <sheets>
     <sheet name="McCauley" sheetId="1" r:id="rId1"/>
     <sheet name="McCauley rotifers" sheetId="5" r:id="rId2"/>
     <sheet name="Bottrell" sheetId="3" r:id="rId3"/>
-    <sheet name="Bottrell pooled" sheetId="4" r:id="rId4"/>
+    <sheet name="bottrell_pooled" sheetId="4" r:id="rId4"/>
     <sheet name="ref" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -3534,7 +3534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0B2460-2955-5C43-9837-B1D9B7377E5B}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4977,8 +4977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970E19EB-C40E-1344-9A19-A1BB7A0CCA20}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Redid how i got the taxonomic hierachy
</commit_message>
<xml_diff>
--- a/Raw_data/master_length_weight.xlsx
+++ b/Raw_data/master_length_weight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF06389-4A1E-694F-A904-059C36AA29F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BBF4AC-D8DD-1649-BAC7-03F6175CCA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
+    <workbookView xWindow="3560" yWindow="740" windowWidth="25840" windowHeight="18380" activeTab="3" xr2:uid="{D745BFE9-FF44-B042-87EE-558B58045933}"/>
   </bookViews>
   <sheets>
     <sheet name="McCauley" sheetId="1" r:id="rId1"/>
@@ -4978,7 +4978,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>